<commit_message>
File read pipeline modification
</commit_message>
<xml_diff>
--- a/My_replacement.xlsx
+++ b/My_replacement.xlsx
@@ -67,42 +67,67 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>330336.0</v>
+          <t>Row transaction type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Replacing Item code</t>
+        </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D1" t="n">
-        <v>303.0</v>
+          <t>Replacing prefix</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Replaced Item code</t>
+        </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>ERA</t>
+          <t>Replaced prefix</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>20220531T1503</t>
-        </is>
-      </c>
-      <c r="G1" t="n">
-        <v>1147.0</v>
-      </c>
-      <c r="H1" t="n">
-        <v>2.0060719E7</v>
-      </c>
-      <c r="I1" t="n">
-        <v>3.27</v>
+          <t>Warehouse code</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Warehouse group code</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Extraction date</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Inherit stock</t>
+        </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>Replacement multiplier</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Replacement Description</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Free text 1</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Free text 2</t>
         </is>
       </c>
     </row>
@@ -133,22 +158,37 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>302.0</v>
+        <v>301.0</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -181,22 +221,37 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>303.0</v>
+        <v>302.0</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -229,22 +284,37 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>304.0</v>
+        <v>303.0</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="J4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -277,22 +347,37 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>305.0</v>
+        <v>304.0</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="J5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -325,22 +410,37 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>306.0</v>
+        <v>305.0</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="J6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -373,22 +473,37 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>310.0</v>
+        <v>306.0</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="J7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -421,22 +536,37 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>320.0</v>
+        <v>310.0</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="J8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -469,22 +599,37 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>321.0</v>
+        <v>320.0</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="J9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -517,22 +662,37 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>322.0</v>
+        <v>321.0</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H10" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="J10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -565,22 +725,37 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>323.0</v>
+        <v>322.0</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H11" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="J11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -613,22 +788,37 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>324.0</v>
+        <v>323.0</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="J12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -661,22 +851,37 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>325.0</v>
+        <v>324.0</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H13" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="J13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -709,22 +914,37 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>333.0</v>
+        <v>325.0</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="J14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -757,22 +977,37 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>350.0</v>
+        <v>333.0</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="J15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -805,22 +1040,37 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>351.0</v>
+        <v>350.0</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="J16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -853,22 +1103,37 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>400.0</v>
+        <v>351.0</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="J17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -901,22 +1166,37 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>651.0</v>
+        <v>400.0</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="J18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -949,22 +1229,37 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>652.0</v>
+        <v>651.0</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H19" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="J19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -997,22 +1292,37 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>653.0</v>
+        <v>652.0</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>1.0</v>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="J20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -1045,22 +1355,100 @@
         </is>
       </c>
       <c r="F21" t="n">
+        <v>653.0</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>566024A</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>566085A</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F22" t="n">
         <v>654.0</v>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H21" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>ERA</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>20220525T1548</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
         <is>
           <t/>
         </is>

</xml_diff>